<commit_message>
Requisitos - Detalles parciales
</commit_message>
<xml_diff>
--- a/Todo/Requisitos/Cronograma.xlsx
+++ b/Todo/Requisitos/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\UdeA\Informática-II-2020-1\ProyectoFinal\Space_Combat_2\Todo\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A82FF2E-F32D-4C41-9EF5-682672782E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16686C3B-50A0-4D4C-8E83-55DE49E68C37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="19770" windowHeight="11760" xr2:uid="{8D4D1FF7-9B20-48EB-A524-C58A5C5D0D9F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Diciembre</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Objetivo, Motivación y Cronograma inicial</t>
+  </si>
+  <si>
+    <t>Planificación, Análisis y repaso de bases</t>
+  </si>
+  <si>
+    <t>Creación de Juego Space Impact 2 en Qt</t>
+  </si>
+  <si>
+    <t>Diseño - Interfaz Gráfica Básica</t>
   </si>
 </sst>
 </file>
@@ -61,7 +70,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,19 +115,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,23 +153,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +487,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A8" sqref="A8"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,216 +497,216 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="2" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
-      <c r="AQ1" s="2"/>
-      <c r="AR1" s="2"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
+      <c r="AM1" s="6"/>
+      <c r="AN1" s="6"/>
+      <c r="AO1" s="6"/>
+      <c r="AP1" s="6"/>
+      <c r="AQ1" s="6"/>
+      <c r="AR1" s="6"/>
+      <c r="AS1" s="6"/>
+      <c r="AT1" s="6"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="1">
         <v>17</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>18</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
         <v>19</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <v>20</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="1">
         <v>21</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="1">
         <v>22</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="1">
         <v>23</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="1">
         <v>24</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="1">
         <v>25</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="1">
         <v>26</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="1">
         <v>27</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="1">
         <v>28</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="1">
         <v>29</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="1">
         <v>30</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="1">
         <v>31</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="2">
         <v>1</v>
       </c>
-      <c r="R2" s="4">
+      <c r="R2" s="2">
         <v>2</v>
       </c>
-      <c r="S2" s="4">
+      <c r="S2" s="2">
         <v>3</v>
       </c>
-      <c r="T2" s="4">
+      <c r="T2" s="2">
         <v>4</v>
       </c>
-      <c r="U2" s="4">
+      <c r="U2" s="2">
         <v>5</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="2">
         <v>6</v>
       </c>
-      <c r="W2" s="4">
+      <c r="W2" s="2">
         <v>7</v>
       </c>
-      <c r="X2" s="4">
+      <c r="X2" s="2">
         <v>8</v>
       </c>
-      <c r="Y2" s="4">
+      <c r="Y2" s="2">
         <v>9</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="Z2" s="2">
         <v>10</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AA2" s="2">
         <v>11</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AB2" s="2">
         <v>12</v>
       </c>
-      <c r="AC2" s="4">
+      <c r="AC2" s="2">
         <v>13</v>
       </c>
-      <c r="AD2" s="4">
+      <c r="AD2" s="2">
         <v>14</v>
       </c>
-      <c r="AE2" s="4">
+      <c r="AE2" s="2">
         <v>15</v>
       </c>
-      <c r="AF2" s="4">
+      <c r="AF2" s="2">
         <v>16</v>
       </c>
-      <c r="AG2" s="4">
+      <c r="AG2" s="2">
         <v>17</v>
       </c>
-      <c r="AH2" s="4">
+      <c r="AH2" s="2">
         <v>18</v>
       </c>
-      <c r="AI2" s="4">
+      <c r="AI2" s="2">
         <v>19</v>
       </c>
-      <c r="AJ2" s="4">
+      <c r="AJ2" s="2">
         <v>20</v>
       </c>
-      <c r="AK2" s="4">
+      <c r="AK2" s="2">
         <v>21</v>
       </c>
-      <c r="AL2" s="4">
+      <c r="AL2" s="2">
         <v>22</v>
       </c>
-      <c r="AM2" s="4">
+      <c r="AM2" s="2">
         <v>23</v>
       </c>
-      <c r="AN2" s="4">
+      <c r="AN2" s="2">
         <v>24</v>
       </c>
-      <c r="AO2" s="4">
+      <c r="AO2" s="2">
         <v>25</v>
       </c>
-      <c r="AP2" s="4">
+      <c r="AP2" s="2">
         <v>26</v>
       </c>
-      <c r="AQ2" s="4">
+      <c r="AQ2" s="2">
         <v>27</v>
       </c>
-      <c r="AR2" s="4">
+      <c r="AR2" s="2">
         <v>28</v>
       </c>
-      <c r="AS2" s="4">
+      <c r="AS2" s="2">
         <v>29</v>
       </c>
-      <c r="AT2" s="4">
+      <c r="AT2" s="2">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
@@ -737,22 +739,24 @@
       <c r="AT3" s="8"/>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
@@ -785,22 +789,24 @@
       <c r="AT4" s="8"/>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
@@ -833,22 +839,24 @@
       <c r="AT5" s="8"/>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
@@ -881,22 +889,22 @@
       <c r="AT6" s="8"/>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
@@ -929,22 +937,22 @@
       <c r="AT7" s="8"/>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
@@ -977,22 +985,22 @@
       <c r="AT8" s="8"/>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
@@ -1025,22 +1033,22 @@
       <c r="AT9" s="8"/>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
       <c r="S10" s="8"/>
@@ -1073,22 +1081,22 @@
       <c r="AT10" s="8"/>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
       <c r="S11" s="8"/>
@@ -1121,22 +1129,22 @@
       <c r="AT11" s="8"/>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
@@ -1169,22 +1177,22 @@
       <c r="AT12" s="8"/>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
@@ -1217,22 +1225,22 @@
       <c r="AT13" s="8"/>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
@@ -1265,22 +1273,22 @@
       <c r="AT14" s="8"/>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
@@ -1313,22 +1321,22 @@
       <c r="AT15" s="8"/>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
@@ -1361,22 +1369,22 @@
       <c r="AT16" s="8"/>
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
@@ -1409,22 +1417,22 @@
       <c r="AT17" s="8"/>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
@@ -1457,22 +1465,22 @@
       <c r="AT18" s="8"/>
     </row>
     <row r="19" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
@@ -1505,22 +1513,22 @@
       <c r="AT19" s="8"/>
     </row>
     <row r="20" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
@@ -1553,22 +1561,22 @@
       <c r="AT20" s="8"/>
     </row>
     <row r="21" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
@@ -1601,22 +1609,22 @@
       <c r="AT21" s="8"/>
     </row>
     <row r="22" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
       <c r="S22" s="8"/>
@@ -1649,22 +1657,22 @@
       <c r="AT22" s="8"/>
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
       <c r="S23" s="8"/>
@@ -1697,22 +1705,22 @@
       <c r="AT23" s="8"/>
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>

</xml_diff>

<commit_message>
Iniciacion de imagenes de niveles
</commit_message>
<xml_diff>
--- a/Todo/Requisitos/Cronograma.xlsx
+++ b/Todo/Requisitos/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\UdeA\Informática-II-2020-1\ProyectoFinal\Space_Combat_2\Todo\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99E805DB-EFAA-4431-A978-9D2E97AC682D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E4F138-2ECF-4489-B8FA-22F7BD8E7D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="19770" windowHeight="11760" xr2:uid="{8D4D1FF7-9B20-48EB-A524-C58A5C5D0D9F}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Diciembre</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>Class Puntos</t>
+  </si>
+  <si>
+    <t>Class Vida</t>
+  </si>
+  <si>
+    <t>Class Paisaje</t>
+  </si>
+  <si>
+    <t>Inicio de niveles construcción basica</t>
+  </si>
+  <si>
+    <t>Diseño de niveles Intermedio</t>
   </si>
 </sst>
 </file>
@@ -130,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,6 +197,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -213,13 +231,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -557,9 +592,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB42B82C-774B-4955-B26D-6D71946914F6}">
-  <dimension ref="A1:AT26"/>
+  <dimension ref="A1:AT29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="E17" sqref="E17"/>
     </sheetView>
@@ -567,203 +602,203 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="46" width="5.28515625" customWidth="1"/>
+    <col min="2" max="46" width="5.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="7" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="7"/>
-      <c r="AG1" s="7"/>
-      <c r="AH1" s="7"/>
-      <c r="AI1" s="7"/>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="7"/>
-      <c r="AL1" s="7"/>
-      <c r="AM1" s="7"/>
-      <c r="AN1" s="7"/>
-      <c r="AO1" s="7"/>
-      <c r="AP1" s="7"/>
-      <c r="AQ1" s="7"/>
-      <c r="AR1" s="7"/>
-      <c r="AS1" s="7"/>
-      <c r="AT1" s="7"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="10"/>
+      <c r="AL1" s="10"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="1">
+      <c r="A2" s="11"/>
+      <c r="B2" s="2">
         <v>17</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>18</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>19</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>20</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>21</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>22</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>23</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="2">
         <v>24</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
         <v>25</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="2">
         <v>26</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="2">
         <v>27</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="2">
         <v>28</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="2">
         <v>29</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="2">
         <v>30</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="2">
         <v>31</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="3">
         <v>1</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="3">
         <v>2</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="3">
         <v>3</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="3">
         <v>4</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="3">
         <v>5</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="3">
         <v>6</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2" s="3">
         <v>7</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="3">
         <v>8</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2" s="3">
         <v>9</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2" s="3">
         <v>10</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA2" s="3">
         <v>11</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AB2" s="3">
         <v>12</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AC2" s="3">
         <v>13</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AD2" s="3">
         <v>14</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AE2" s="3">
         <v>15</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AF2" s="3">
         <v>16</v>
       </c>
-      <c r="AG2" s="2">
+      <c r="AG2" s="3">
         <v>17</v>
       </c>
-      <c r="AH2" s="2">
+      <c r="AH2" s="3">
         <v>18</v>
       </c>
-      <c r="AI2" s="2">
+      <c r="AI2" s="3">
         <v>19</v>
       </c>
-      <c r="AJ2" s="2">
+      <c r="AJ2" s="3">
         <v>20</v>
       </c>
-      <c r="AK2" s="2">
+      <c r="AK2" s="3">
         <v>21</v>
       </c>
-      <c r="AL2" s="2">
+      <c r="AL2" s="3">
         <v>22</v>
       </c>
-      <c r="AM2" s="2">
+      <c r="AM2" s="3">
         <v>23</v>
       </c>
-      <c r="AN2" s="2">
+      <c r="AN2" s="3">
         <v>24</v>
       </c>
-      <c r="AO2" s="2">
+      <c r="AO2" s="3">
         <v>25</v>
       </c>
-      <c r="AP2" s="2">
+      <c r="AP2" s="3">
         <v>26</v>
       </c>
-      <c r="AQ2" s="2">
+      <c r="AQ2" s="3">
         <v>27</v>
       </c>
-      <c r="AR2" s="2">
+      <c r="AR2" s="3">
         <v>28</v>
       </c>
-      <c r="AS2" s="2">
+      <c r="AS2" s="3">
         <v>29</v>
       </c>
-      <c r="AT2" s="2">
+      <c r="AT2" s="3">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4"/>
@@ -813,7 +848,7 @@
       <c r="AT3" s="5"/>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5"/>
@@ -863,7 +898,7 @@
       <c r="AT4" s="5"/>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="5"/>
@@ -871,7 +906,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -913,7 +948,7 @@
       <c r="AT5" s="5"/>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="5"/>
@@ -921,7 +956,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -963,7 +998,7 @@
       <c r="AT6" s="5"/>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="5"/>
@@ -971,7 +1006,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -1013,7 +1048,7 @@
       <c r="AT7" s="5"/>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="5"/>
@@ -1021,7 +1056,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="4"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -1063,7 +1098,7 @@
       <c r="AT8" s="5"/>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="5"/>
@@ -1072,7 +1107,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="H9" s="4"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -1113,7 +1148,7 @@
       <c r="AT9" s="5"/>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="5"/>
@@ -1122,7 +1157,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="H10" s="4"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -1163,7 +1198,7 @@
       <c r="AT10" s="5"/>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="5"/>
@@ -1172,7 +1207,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="H11" s="4"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -1213,7 +1248,7 @@
       <c r="AT11" s="5"/>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="5"/>
@@ -1222,7 +1257,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="H12" s="4"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -1263,7 +1298,7 @@
       <c r="AT12" s="5"/>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="5"/>
@@ -1273,7 +1308,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
@@ -1313,7 +1348,7 @@
       <c r="AT13" s="5"/>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="5"/>
@@ -1323,7 +1358,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="I14" s="4"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -1363,8 +1398,8 @@
       <c r="AT14" s="5"/>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>12</v>
+      <c r="A15" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1373,7 +1408,7 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="4"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -1413,8 +1448,8 @@
       <c r="AT15" s="5"/>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>13</v>
+      <c r="A16" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1424,7 +1459,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="J16" s="4"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -1463,8 +1498,8 @@
       <c r="AT16" s="5"/>
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>14</v>
+      <c r="A17" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1474,9 +1509,9 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="4"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -1513,8 +1548,8 @@
       <c r="AT17" s="5"/>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>18</v>
+      <c r="A18" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1526,7 +1561,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="L18" s="7"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
@@ -1563,8 +1598,8 @@
       <c r="AT18" s="5"/>
     </row>
     <row r="19" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>17</v>
+      <c r="A19" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1576,7 +1611,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
+      <c r="L19" s="4"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
@@ -1613,8 +1648,8 @@
       <c r="AT19" s="5"/>
     </row>
     <row r="20" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>20</v>
+      <c r="A20" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1626,7 +1661,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
+      <c r="L20" s="7"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
@@ -1634,7 +1669,7 @@
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
+      <c r="T20" s="4"/>
       <c r="U20" s="5"/>
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
@@ -1663,7 +1698,9 @@
       <c r="AT20" s="5"/>
     </row>
     <row r="21" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1674,7 +1711,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
+      <c r="L21" s="8"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -1682,8 +1719,8 @@
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="4"/>
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
       <c r="X21" s="5"/>
@@ -1711,7 +1748,9 @@
       <c r="AT21" s="5"/>
     </row>
     <row r="22" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1731,7 +1770,7 @@
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
+      <c r="U22" s="4"/>
       <c r="V22" s="5"/>
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
@@ -1759,7 +1798,9 @@
       <c r="AT22" s="5"/>
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1779,7 +1820,7 @@
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
+      <c r="U23" s="4"/>
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
       <c r="X23" s="5"/>
@@ -1807,7 +1848,9 @@
       <c r="AT23" s="5"/>
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1855,7 +1898,7 @@
       <c r="AT24" s="5"/>
     </row>
     <row r="25" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="A25" s="1"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -1903,7 +1946,7 @@
       <c r="AT25" s="5"/>
     </row>
     <row r="26" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="A26" s="1"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1949,6 +1992,150 @@
       <c r="AR26" s="5"/>
       <c r="AS26" s="5"/>
       <c r="AT26" s="5"/>
+    </row>
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
+      <c r="AF27" s="5"/>
+      <c r="AG27" s="5"/>
+      <c r="AH27" s="5"/>
+      <c r="AI27" s="5"/>
+      <c r="AJ27" s="5"/>
+      <c r="AK27" s="5"/>
+      <c r="AL27" s="5"/>
+      <c r="AM27" s="5"/>
+      <c r="AN27" s="5"/>
+      <c r="AO27" s="5"/>
+      <c r="AP27" s="5"/>
+      <c r="AQ27" s="5"/>
+      <c r="AR27" s="5"/>
+      <c r="AS27" s="5"/>
+      <c r="AT27" s="5"/>
+    </row>
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+      <c r="AF28" s="5"/>
+      <c r="AG28" s="5"/>
+      <c r="AH28" s="5"/>
+      <c r="AI28" s="5"/>
+      <c r="AJ28" s="5"/>
+      <c r="AK28" s="5"/>
+      <c r="AL28" s="5"/>
+      <c r="AM28" s="5"/>
+      <c r="AN28" s="5"/>
+      <c r="AO28" s="5"/>
+      <c r="AP28" s="5"/>
+      <c r="AQ28" s="5"/>
+      <c r="AR28" s="5"/>
+      <c r="AS28" s="5"/>
+      <c r="AT28" s="5"/>
+    </row>
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="5"/>
+      <c r="AG29" s="5"/>
+      <c r="AH29" s="5"/>
+      <c r="AI29" s="5"/>
+      <c r="AJ29" s="5"/>
+      <c r="AK29" s="5"/>
+      <c r="AL29" s="5"/>
+      <c r="AM29" s="5"/>
+      <c r="AN29" s="5"/>
+      <c r="AO29" s="5"/>
+      <c r="AP29" s="5"/>
+      <c r="AQ29" s="5"/>
+      <c r="AR29" s="5"/>
+      <c r="AS29" s="5"/>
+      <c r="AT29" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2111,14 +2298,14 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C016673-77F8-4AD7-92C1-CABDAD548F4D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="0da812b4-49a8-4424-af0f-96ea194d4538"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0da812b4-49a8-4424-af0f-96ea194d4538"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
detalles y mas analisis
</commit_message>
<xml_diff>
--- a/Todo/Requisitos/Cronograma.xlsx
+++ b/Todo/Requisitos/Cronograma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\UdeA\Informática-II-2020-1\ProyectoFinal\Space_Combat_2\Todo\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E4F138-2ECF-4489-B8FA-22F7BD8E7D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AF9102-1710-4C58-B298-485CC6E08EE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="19770" windowHeight="11760" xr2:uid="{8D4D1FF7-9B20-48EB-A524-C58A5C5D0D9F}"/>
   </bookViews>
@@ -594,9 +594,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB42B82C-774B-4955-B26D-6D71946914F6}">
   <dimension ref="A1:AT29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E17" sqref="E17"/>
+      <selection pane="topRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,7 +1873,7 @@
       <c r="U24" s="5"/>
       <c r="V24" s="5"/>
       <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
+      <c r="X24" s="7"/>
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
@@ -2149,21 +2149,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001A62D2D66987B640A3C59AF3994AF467" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="137f91acb5bcc5fe6bdd21676251dd10">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0da812b4-49a8-4424-af0f-96ea194d4538" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4b8f4c84b2e19a15e630d30243e6cde" ns3:_="">
     <xsd:import namespace="0da812b4-49a8-4424-af0f-96ea194d4538"/>
@@ -2295,31 +2280,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C016673-77F8-4AD7-92C1-CABDAD548F4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0da812b4-49a8-4424-af0f-96ea194d4538"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D1B572-887F-4494-9E99-88F43967F978}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3AB878CA-2CB8-4048-8D05-0999E1EE839B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2335,4 +2311,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D1B572-887F-4494-9E99-88F43967F978}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C016673-77F8-4AD7-92C1-CABDAD548F4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0da812b4-49a8-4424-af0f-96ea194d4538"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
organizacion de niveles avanzado 2, basico
</commit_message>
<xml_diff>
--- a/Todo/Requisitos/Cronograma.xlsx
+++ b/Todo/Requisitos/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\UdeA\Informática-II-2020-1\ProyectoFinal\Space_Combat_2\Todo\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AF9102-1710-4C58-B298-485CC6E08EE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B99138E-E501-48E9-A1D3-6935CB62C936}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="19770" windowHeight="11760" xr2:uid="{8D4D1FF7-9B20-48EB-A524-C58A5C5D0D9F}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Diciembre</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Diseño de niveles Intermedio</t>
+  </si>
+  <si>
+    <t>Diseño de niveles Avanzado 1</t>
+  </si>
+  <si>
+    <t>Diseño de niveles Avanzado 2</t>
   </si>
 </sst>
 </file>
@@ -594,9 +600,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB42B82C-774B-4955-B26D-6D71946914F6}">
   <dimension ref="A1:AT29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,7 +1880,7 @@
       <c r="V24" s="5"/>
       <c r="W24" s="5"/>
       <c r="X24" s="7"/>
-      <c r="Y24" s="5"/>
+      <c r="Y24" s="4"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
       <c r="AB24" s="5"/>
@@ -1898,7 +1904,9 @@
       <c r="AT24" s="5"/>
     </row>
     <row r="25" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -1922,8 +1930,8 @@
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
-      <c r="Z25" s="5"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="4"/>
       <c r="AA25" s="5"/>
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
@@ -1946,7 +1954,9 @@
       <c r="AT25" s="5"/>
     </row>
     <row r="26" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>

</xml_diff>

<commit_message>
Inicio de menu, basico e intermedio
</commit_message>
<xml_diff>
--- a/Todo/Requisitos/Cronograma.xlsx
+++ b/Todo/Requisitos/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\UdeA\Informática-II-2020-1\ProyectoFinal\Space_Combat_2\Todo\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B99138E-E501-48E9-A1D3-6935CB62C936}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB041BE5-DFC1-43C9-9851-56F56E7BB54C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="19770" windowHeight="11760" xr2:uid="{8D4D1FF7-9B20-48EB-A524-C58A5C5D0D9F}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Diciembre</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>Diseño de niveles Avanzado 2</t>
+  </si>
+  <si>
+    <t>Menú basico</t>
+  </si>
+  <si>
+    <t>Menú intermedio</t>
+  </si>
+  <si>
+    <t>Menú avanzado</t>
   </si>
 </sst>
 </file>
@@ -600,9 +609,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB42B82C-774B-4955-B26D-6D71946914F6}">
   <dimension ref="A1:AT29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AP28" sqref="AP28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,7 +1990,7 @@
       <c r="W26" s="5"/>
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
-      <c r="Z26" s="5"/>
+      <c r="Z26" s="4"/>
       <c r="AA26" s="5"/>
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
@@ -2004,7 +2013,9 @@
       <c r="AT26" s="5"/>
     </row>
     <row r="27" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -2044,15 +2055,17 @@
       <c r="AL27" s="5"/>
       <c r="AM27" s="5"/>
       <c r="AN27" s="5"/>
-      <c r="AO27" s="5"/>
-      <c r="AP27" s="5"/>
+      <c r="AO27" s="7"/>
+      <c r="AP27" s="7"/>
       <c r="AQ27" s="5"/>
       <c r="AR27" s="5"/>
       <c r="AS27" s="5"/>
       <c r="AT27" s="5"/>
     </row>
     <row r="28" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -2100,7 +2113,9 @@
       <c r="AT28" s="5"/>
     </row>
     <row r="29" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -2159,6 +2174,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001A62D2D66987B640A3C59AF3994AF467" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="137f91acb5bcc5fe6bdd21676251dd10">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0da812b4-49a8-4424-af0f-96ea194d4538" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4b8f4c84b2e19a15e630d30243e6cde" ns3:_="">
     <xsd:import namespace="0da812b4-49a8-4424-af0f-96ea194d4538"/>
@@ -2290,22 +2320,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C016673-77F8-4AD7-92C1-CABDAD548F4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0da812b4-49a8-4424-af0f-96ea194d4538"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D1B572-887F-4494-9E99-88F43967F978}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3AB878CA-2CB8-4048-8D05-0999E1EE839B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2321,28 +2360,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D1B572-887F-4494-9E99-88F43967F978}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C016673-77F8-4AD7-92C1-CABDAD548F4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0da812b4-49a8-4424-af0f-96ea194d4538"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Menu - Inicio y cargar
</commit_message>
<xml_diff>
--- a/Todo/Requisitos/Cronograma.xlsx
+++ b/Todo/Requisitos/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\UdeA\Informática-II-2020-1\ProyectoFinal\Space_Combat_2\Todo\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB041BE5-DFC1-43C9-9851-56F56E7BB54C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C553B8-3DBD-44D4-A4DD-7C94E3467BD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="19770" windowHeight="11760" xr2:uid="{8D4D1FF7-9B20-48EB-A524-C58A5C5D0D9F}"/>
   </bookViews>
@@ -609,9 +609,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB42B82C-774B-4955-B26D-6D71946914F6}">
   <dimension ref="A1:AT29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AP28" sqref="AP28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AN27" sqref="AA27:AN27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,8 +2107,8 @@
       <c r="AN28" s="5"/>
       <c r="AO28" s="5"/>
       <c r="AP28" s="5"/>
-      <c r="AQ28" s="5"/>
-      <c r="AR28" s="5"/>
+      <c r="AQ28" s="7"/>
+      <c r="AR28" s="4"/>
       <c r="AS28" s="5"/>
       <c r="AT28" s="5"/>
     </row>
@@ -2158,7 +2158,7 @@
       <c r="AO29" s="5"/>
       <c r="AP29" s="5"/>
       <c r="AQ29" s="5"/>
-      <c r="AR29" s="5"/>
+      <c r="AR29" s="7"/>
       <c r="AS29" s="5"/>
       <c r="AT29" s="5"/>
     </row>
@@ -2174,21 +2174,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001A62D2D66987B640A3C59AF3994AF467" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="137f91acb5bcc5fe6bdd21676251dd10">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0da812b4-49a8-4424-af0f-96ea194d4538" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4b8f4c84b2e19a15e630d30243e6cde" ns3:_="">
     <xsd:import namespace="0da812b4-49a8-4424-af0f-96ea194d4538"/>
@@ -2320,31 +2305,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C016673-77F8-4AD7-92C1-CABDAD548F4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0da812b4-49a8-4424-af0f-96ea194d4538"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D1B572-887F-4494-9E99-88F43967F978}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3AB878CA-2CB8-4048-8D05-0999E1EE839B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2360,4 +2336,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D1B572-887F-4494-9E99-88F43967F978}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C016673-77F8-4AD7-92C1-CABDAD548F4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0da812b4-49a8-4424-af0f-96ea194d4538"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Finalizacion basica de menu avanzado
</commit_message>
<xml_diff>
--- a/Todo/Requisitos/Cronograma.xlsx
+++ b/Todo/Requisitos/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\UdeA\Informática-II-2020-1\ProyectoFinal\Space_Combat_2\Todo\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C553B8-3DBD-44D4-A4DD-7C94E3467BD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1878701-DDA2-4563-BC00-B982CB60601E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="19770" windowHeight="11760" xr2:uid="{8D4D1FF7-9B20-48EB-A524-C58A5C5D0D9F}"/>
   </bookViews>
@@ -609,9 +609,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB42B82C-774B-4955-B26D-6D71946914F6}">
   <dimension ref="A1:AT29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AN27" sqref="AA27:AN27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AT30" sqref="AT30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2159,7 +2159,7 @@
       <c r="AP29" s="5"/>
       <c r="AQ29" s="5"/>
       <c r="AR29" s="7"/>
-      <c r="AS29" s="5"/>
+      <c r="AS29" s="4"/>
       <c r="AT29" s="5"/>
     </row>
   </sheetData>
@@ -2174,6 +2174,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001A62D2D66987B640A3C59AF3994AF467" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="137f91acb5bcc5fe6bdd21676251dd10">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0da812b4-49a8-4424-af0f-96ea194d4538" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4b8f4c84b2e19a15e630d30243e6cde" ns3:_="">
     <xsd:import namespace="0da812b4-49a8-4424-af0f-96ea194d4538"/>
@@ -2305,22 +2320,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C016673-77F8-4AD7-92C1-CABDAD548F4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0da812b4-49a8-4424-af0f-96ea194d4538"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D1B572-887F-4494-9E99-88F43967F978}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3AB878CA-2CB8-4048-8D05-0999E1EE839B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2336,28 +2360,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D1B572-887F-4494-9E99-88F43967F978}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C016673-77F8-4AD7-92C1-CABDAD548F4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0da812b4-49a8-4424-af0f-96ea194d4538"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
conexion de menu y juego
</commit_message>
<xml_diff>
--- a/Todo/Requisitos/Cronograma.xlsx
+++ b/Todo/Requisitos/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\UdeA\Informática-II-2020-1\ProyectoFinal\Space_Combat_2\Todo\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1878701-DDA2-4563-BC00-B982CB60601E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036C26E9-D952-4C89-A73E-C5BCE693866E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="19770" windowHeight="11760" xr2:uid="{8D4D1FF7-9B20-48EB-A524-C58A5C5D0D9F}"/>
   </bookViews>
@@ -609,9 +609,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB42B82C-774B-4955-B26D-6D71946914F6}">
   <dimension ref="A1:AT29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AT30" sqref="AT30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q1" sqref="Q1:AT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2174,21 +2174,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001A62D2D66987B640A3C59AF3994AF467" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="137f91acb5bcc5fe6bdd21676251dd10">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0da812b4-49a8-4424-af0f-96ea194d4538" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4b8f4c84b2e19a15e630d30243e6cde" ns3:_="">
     <xsd:import namespace="0da812b4-49a8-4424-af0f-96ea194d4538"/>
@@ -2320,31 +2305,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C016673-77F8-4AD7-92C1-CABDAD548F4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0da812b4-49a8-4424-af0f-96ea194d4538"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D1B572-887F-4494-9E99-88F43967F978}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3AB878CA-2CB8-4048-8D05-0999E1EE839B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2360,4 +2336,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D1B572-887F-4494-9E99-88F43967F978}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C016673-77F8-4AD7-92C1-CABDAD548F4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0da812b4-49a8-4424-af0f-96ea194d4538"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>